<commit_message>
try using static middleware
</commit_message>
<xml_diff>
--- a/old_ref/X50/output/summary0705.xlsx
+++ b/old_ref/X50/output/summary0705.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dimsp\Documents\Projects\nodejsLearning\tdtoolkit_web\old_ref\X50\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB97D80-4741-4ABB-9C58-9AE15905CDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="39">
   <si>
     <t>LC</t>
   </si>
@@ -141,18 +135,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Eab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>todo</t>
+  </si>
+  <si>
+    <t>Ea</t>
+  </si>
+  <si>
+    <t>Eb</t>
+  </si>
+  <si>
+    <t>ΔEab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -228,7 +230,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -301,7 +303,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -353,7 +355,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -547,21 +549,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="AF1" activeCellId="1" sqref="A1:P2 R1:AF2 A6:P7 R6:AF7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="2" width="11.5703125" style="1"/>
     <col min="3" max="7" width="12.28515625" style="1" customWidth="1"/>
@@ -570,7 +572,7 @@
     <col min="18" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -625,10 +627,14 @@
       <c r="S1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
+      <c r="T1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="V1" s="7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="W1" s="2" t="s">
         <v>14</v>
@@ -661,7 +667,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="12" customHeight="1">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -671,10 +677,18 @@
       <c r="C2" s="3">
         <v>6515</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="H2" s="3">
         <v>5.18</v>
       </c>
@@ -705,11 +719,21 @@
       <c r="Q2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
+      <c r="R2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="W2" s="3">
         <v>1410.8</v>
       </c>
@@ -741,7 +765,7 @@
         <v>15.57</v>
       </c>
     </row>
-    <row r="3" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" hidden="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -751,10 +775,18 @@
       <c r="C3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="H3" s="3" t="s">
         <v>22</v>
       </c>
@@ -783,11 +815,21 @@
       <c r="Q3" s="3">
         <v>75.8</v>
       </c>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
+      <c r="R3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="W3" s="3">
         <v>1419</v>
       </c>
@@ -813,7 +855,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" ht="27" hidden="1">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -822,6 +864,18 @@
       </c>
       <c r="C4" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="H4" s="4">
         <v>4.8</v>
@@ -855,6 +909,21 @@
       <c r="Q4" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="R4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="W4" s="1">
         <f>W2*AB4/AA4</f>
         <v>1321.0218181818182</v>
@@ -889,7 +958,7 @@
         <v>17.089322752985545</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" hidden="1">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -898,6 +967,18 @@
       </c>
       <c r="C5" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="H5" s="4">
         <v>4.8</v>
@@ -929,6 +1010,21 @@
         <f t="shared" ref="P5:P7" si="1">O5-$O$2</f>
         <v>2.4675000000000002E-2</v>
       </c>
+      <c r="R5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="W5" s="1">
         <f>$W$2*AB5/AA5</f>
         <v>982.08391156775883</v>
@@ -963,7 +1059,7 @@
         <v>17.431843180389691</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" ht="14.25" customHeight="1">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -972,6 +1068,18 @@
       </c>
       <c r="C6" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="H6" s="1">
         <v>5.08</v>
@@ -1002,6 +1110,21 @@
         <f t="shared" si="1"/>
         <v>-3.1249999999999889E-3</v>
       </c>
+      <c r="R6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="W6" s="1">
         <f>$W$2*AB6/AA6</f>
         <v>1341.6896953893565</v>
@@ -1035,7 +1158,7 @@
         <v>15.792638277812697</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -1044,6 +1167,18 @@
       </c>
       <c r="C7" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="H7" s="1">
         <v>5.08</v>
@@ -1075,6 +1210,21 @@
         <f t="shared" si="1"/>
         <v>2.1274999999999988E-2</v>
       </c>
+      <c r="R7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="W7" s="1">
         <f>$W$2*AB7/AA7</f>
         <v>967.62722356924633</v>
@@ -1108,7 +1258,7 @@
         <v>18.728527655562541</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32">
       <c r="L8" s="6" t="s">
         <v>32</v>
       </c>

</xml_diff>